<commit_message>
Excel Update + Accessory Images
</commit_message>
<xml_diff>
--- a/MIE350 Data import.xlsx
+++ b/MIE350 Data import.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Dropbox\University\Year 3\3F\MIE350 - Design and Analysis of Information Systems\Project\MIE350Proj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kait L\Documents\GitHub\MIE350Proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514A4721-9940-4B18-A542-ABDFC67A43E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B5270F-164C-41C9-8B30-C6BCB9E8D38A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Video_games" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="248">
   <si>
     <t>Super Mario Odyssey</t>
   </si>
@@ -702,6 +702,84 @@
   </si>
   <si>
     <t>Max_Players</t>
+  </si>
+  <si>
+    <t>Image File Name</t>
+  </si>
+  <si>
+    <t>Switch_SuperMarioOdyssey.jpg</t>
+  </si>
+  <si>
+    <t>Switch_BreathOfTheWild.jpg</t>
+  </si>
+  <si>
+    <t>Switch_ThreeHouses.jpg</t>
+  </si>
+  <si>
+    <t>Switch_SuperMarioMaker2.jpg</t>
+  </si>
+  <si>
+    <t>Switch_LinksAwakening.jpg</t>
+  </si>
+  <si>
+    <t>Switch_SuperSmashBrosUltimate.jpg</t>
+  </si>
+  <si>
+    <t>3ds_Awakening.jpg</t>
+  </si>
+  <si>
+    <t>3ds_KirbysEpicYarn.jpg</t>
+  </si>
+  <si>
+    <t>3ds_MajorasMask3D.jpg</t>
+  </si>
+  <si>
+    <t>3ds_MarioKart7.jpg</t>
+  </si>
+  <si>
+    <t>3ds_FederationForce.jpg</t>
+  </si>
+  <si>
+    <t>Ps4_Persona5.jpg</t>
+  </si>
+  <si>
+    <t>Ps4_TrailsOfColdSteel3.jpg</t>
+  </si>
+  <si>
+    <t>Ps4_TheSims4.jpg</t>
+  </si>
+  <si>
+    <t>Ps4_KingdomHearts3.jpg</t>
+  </si>
+  <si>
+    <t>Xbox_Nba2k20.jpg</t>
+  </si>
+  <si>
+    <t>Psvita_Persona4Golden.jpg</t>
+  </si>
+  <si>
+    <t>Psvita_MetalGearSolid.jpg</t>
+  </si>
+  <si>
+    <t>Psvita_MostWanted.jpg</t>
+  </si>
+  <si>
+    <t>Psvita_BlackOpsDeclassified.jpg</t>
+  </si>
+  <si>
+    <t>Accessory_Psvita.jpg</t>
+  </si>
+  <si>
+    <t>Accessory_3ds.jpg</t>
+  </si>
+  <si>
+    <t>Accessory_Xbox.jpg</t>
+  </si>
+  <si>
+    <t>Accessory_Switch.jpg</t>
+  </si>
+  <si>
+    <t>Accessory_Ps4.jpg</t>
   </si>
 </sst>
 </file>
@@ -777,7 +855,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -785,11 +863,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -810,29 +903,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1015,6 +1093,24 @@
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1029,20 +1125,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D6D04670-FF85-4C72-A279-1207C4AE2208}" name="Table1" displayName="Table1" ref="A1:K21" totalsRowShown="0" dataDxfId="0">
-  <autoFilter ref="A1:K21" xr:uid="{64C99CD8-8F73-4AF1-8C88-49FBB0E1F7C3}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{3942920C-0B16-4A93-8F94-4F88D5EEE647}" name="UPC" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{54C084C1-0165-4848-8070-A36076F1FB12}" name="Title" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{FE526B94-BD66-4984-A443-2A7514CFC30B}" name="Developer" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{086A04FE-945C-40B2-A4C1-BCA43F4425A7}" name="Console" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{03E24877-D928-4354-98AB-FA1DCD1F60D1}" name="Genre" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{DE1A730D-E6E5-44A2-872D-A4792C0EAF16}" name="Release_Date" dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D6D04670-FF85-4C72-A279-1207C4AE2208}" name="Table1" displayName="Table1" ref="A1:L21" totalsRowShown="0" dataDxfId="10">
+  <autoFilter ref="A1:L21" xr:uid="{64C99CD8-8F73-4AF1-8C88-49FBB0E1F7C3}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{3942920C-0B16-4A93-8F94-4F88D5EEE647}" name="UPC" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{54C084C1-0165-4848-8070-A36076F1FB12}" name="Title" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{FE526B94-BD66-4984-A443-2A7514CFC30B}" name="Developer" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{086A04FE-945C-40B2-A4C1-BCA43F4425A7}" name="Console" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{03E24877-D928-4354-98AB-FA1DCD1F60D1}" name="Genre" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{DE1A730D-E6E5-44A2-872D-A4792C0EAF16}" name="Release_Date" dataDxfId="4"/>
     <tableColumn id="7" xr3:uid="{3A342EC6-80C1-42E4-8CF4-CEF1CB954027}" name="Consumer_Rating"/>
-    <tableColumn id="8" xr3:uid="{3F488593-1DB6-407B-A6B3-761443AB8C0F}" name="ESRB_Rating" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{0ED7A100-E064-47C0-9E04-59C291F39908}" name="Price" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{084B7F2C-CA25-4777-9B82-E45D99F2CAE6}" name="Description" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{4F826A71-2188-4ACF-A09A-2668F88DDACE}" name="Max_Players" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{3F488593-1DB6-407B-A6B3-761443AB8C0F}" name="ESRB_Rating" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{0ED7A100-E064-47C0-9E04-59C291F39908}" name="Price" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{084B7F2C-CA25-4777-9B82-E45D99F2CAE6}" name="Description" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{4F826A71-2188-4ACF-A09A-2668F88DDACE}" name="Max_Players" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{374F5240-3EC5-4547-AD0A-AF81131E1230}" name="Image File Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1311,26 +1408,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" customWidth="1"/>
-    <col min="6" max="6" width="17.08984375" customWidth="1"/>
-    <col min="7" max="7" width="17.40625" customWidth="1"/>
-    <col min="8" max="8" width="13.08984375" customWidth="1"/>
-    <col min="10" max="10" width="255.58984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.2265625" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="64.140625" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" customWidth="1"/>
+    <col min="12" max="12" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>216</v>
       </c>
@@ -1364,8 +1463,11 @@
       <c r="K1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1">
       <c r="A2" s="1">
         <v>45496590741</v>
       </c>
@@ -1399,8 +1501,11 @@
       <c r="K2" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2" s="14" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1">
       <c r="A3" s="1">
         <v>45496590420</v>
       </c>
@@ -1434,8 +1539,11 @@
       <c r="K3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3" s="14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1">
       <c r="A4" s="1">
         <v>45496593858</v>
       </c>
@@ -1469,8 +1577,11 @@
       <c r="K4" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="L4" s="14" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" thickBot="1">
       <c r="A5" s="1">
         <v>45496596484</v>
       </c>
@@ -1504,8 +1615,11 @@
       <c r="K5" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5" s="14" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" thickBot="1">
       <c r="A6" s="1">
         <v>4549659655</v>
       </c>
@@ -1539,8 +1653,11 @@
       <c r="K6" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6" s="14" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" thickBot="1">
       <c r="A7" s="12">
         <v>45496422899</v>
       </c>
@@ -1574,8 +1691,11 @@
       <c r="K7" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7" s="14" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1">
       <c r="A8" s="1">
         <v>21112248920</v>
       </c>
@@ -1609,8 +1729,11 @@
       <c r="K8" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="L8" s="14" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" thickBot="1">
       <c r="A9" s="1">
         <v>45496901998</v>
       </c>
@@ -1644,8 +1767,11 @@
       <c r="K9" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9" s="14" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" thickBot="1">
       <c r="A10" s="1">
         <v>45496742805</v>
       </c>
@@ -1679,8 +1805,11 @@
       <c r="K10" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L10" s="14" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" thickBot="1">
       <c r="A11" s="1">
         <v>45496741747</v>
       </c>
@@ -1714,8 +1843,11 @@
       <c r="K11" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L11" s="14" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" thickBot="1">
       <c r="A12" s="13">
         <v>45496743888</v>
       </c>
@@ -1749,8 +1881,11 @@
       <c r="K12" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="L12" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" thickBot="1">
       <c r="A13" s="1">
         <v>730865020102</v>
       </c>
@@ -1784,8 +1919,11 @@
       <c r="K13" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="L13" s="14" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1">
       <c r="A14" s="1">
         <v>810023033219</v>
       </c>
@@ -1819,8 +1957,11 @@
       <c r="K14" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="L14" s="14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" thickBot="1">
       <c r="A15" s="12">
         <v>14633738179</v>
       </c>
@@ -1854,8 +1995,11 @@
       <c r="K15" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="L15" s="14" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" thickBot="1">
       <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
@@ -1889,8 +2033,11 @@
       <c r="K16" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L16" s="14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" thickBot="1">
       <c r="A17" s="1">
         <v>71042559529</v>
       </c>
@@ -1924,8 +2071,11 @@
       <c r="K17" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17" s="14" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" thickBot="1">
       <c r="A18" s="1">
         <v>730865200009</v>
       </c>
@@ -1959,8 +2109,11 @@
       <c r="K18" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18" s="14" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" thickBot="1">
       <c r="A19" s="13">
         <v>83717202394</v>
       </c>
@@ -1994,8 +2147,11 @@
       <c r="K19" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="L19" s="14" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" thickBot="1">
       <c r="A20" s="13">
         <v>14633354522</v>
       </c>
@@ -2029,8 +2185,11 @@
       <c r="K20" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="L20" s="14" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>73</v>
       </c>
@@ -2064,29 +2223,36 @@
       <c r="K21" s="2">
         <v>4</v>
       </c>
+      <c r="L21" s="14" t="s">
+        <v>242</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8109F163-36B7-476B-AE41-C30DA12AB517}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.6796875" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>130</v>
       </c>
@@ -2102,8 +2268,11 @@
       <c r="E1" s="5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="7" t="s">
         <v>79</v>
       </c>
@@ -2119,8 +2288,11 @@
       <c r="E2" s="5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>711719504405</v>
       </c>
@@ -2136,8 +2308,11 @@
       <c r="E3" s="8" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>85</v>
       </c>
@@ -2153,8 +2328,11 @@
       <c r="E4" s="8" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="7" t="s">
         <v>88</v>
       </c>
@@ -2169,6 +2347,9 @@
       </c>
       <c r="E5" s="2" t="s">
         <v>90</v>
+      </c>
+      <c r="F5" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -2184,7 +2365,7 @@
       <selection sqref="A1:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="2">
@@ -2359,7 +2540,7 @@
       <selection sqref="A1:C125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -3749,7 +3930,7 @@
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
@@ -3827,9 +4008,9 @@
       <selection activeCell="C61" sqref="C61:C63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.6796875" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>